<commit_message>
MNIST : He initializer
</commit_message>
<xml_diff>
--- a/1_MNIST/DL_Lecture/Evaluation result_Homework1.xlsx
+++ b/1_MNIST/DL_Lecture/Evaluation result_Homework1.xlsx
@@ -19,11 +19,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<x:sst xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
   <x:si>
     <x:t>adam</x:t>
   </x:si>
   <x:si>
+    <x:t>Setting#3</x:t>
+  </x:si>
+  <x:si>
     <x:t>Learning rate</x:t>
   </x:si>
   <x:si>
@@ -36,9 +39,6 @@
     <x:t>3.45 minutes</x:t>
   </x:si>
   <x:si>
-    <x:t>Setting #1 다른 설정과 비교하기 위한 기준점(Baseline)으로, 추가 기법 없이 기본 파라미터로만 학습 Setting#2 기준점에서 Layer 개수를 4개로 확장</x:t>
-  </x:si>
-  <x:si>
     <x:t>Xavier Normal</x:t>
   </x:si>
   <x:si>
@@ -99,6 +99,11 @@
     <x:t>…</x:t>
   </x:si>
   <x:si>
+    <x:t>Setting #1 다른 설정과 비교하기 위한 기준점(Baseline)으로, 추가 기법 없이 기본 파라미터로만 학습
+ Setting#2 기준점에서 Layer 개수를 4개로 확장 
+Setting #3 (Setting#3에서 dropout 0.5 를 적용)</x:t>
+  </x:si>
+  <x:si>
     <x:t>None</x:t>
   </x:si>
   <x:si>
@@ -106,6 +111,9 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">(300 → 200 → 100 → 10)	</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3.36 minutes</x:t>
   </x:si>
   <x:si>
     <x:t>ReLU</x:t>
@@ -396,7 +404,7 @@
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="35">
+  <x:cellXfs count="36">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <x:alignment horizontal="general" vertical="center"/>
     </x:xf>
@@ -742,6 +750,19 @@
         </x:xf>
       </mc:Fallback>
     </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:hs="http://schemas.haansoft.com/office/spreadsheet/8.0" Requires="hs">
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" hs:applyExtension="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+          <hs:parashape hs:lineSpacingType="betweenLines" hs:lineSpacing="75" hs:breakNonLatinWord="breakWord" hs:breakLatinWord="keepWord" hs:condense="0" hs:textAlignment="baseLine"/>
+        </x:xf>
+      </mc:Choice>
+      <mc:Fallback>
+        <x:xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+          <x:alignment horizontal="center" vertical="center" wrapText="1"/>
+        </x:xf>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </x:cellXfs>
   <x:cellStyles count="1">
     <x:cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -751,7 +772,7 @@
 </x:styleSheet>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1195,7 +1216,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1341320" y="8962625"/>
+          <a:off x="1343025" y="8963025"/>
           <a:ext cx="7178792" cy="2895700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1233,7 +1254,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9354926" y="8962625"/>
+          <a:off x="9353550" y="8963025"/>
           <a:ext cx="6572384" cy="2705603"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1271,7 +1292,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9344024" y="11763879"/>
+          <a:off x="9344025" y="11763375"/>
           <a:ext cx="6583287" cy="2588152"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1309,8 +1330,84 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1341320" y="11763879"/>
+          <a:off x="1343025" y="11763375"/>
           <a:ext cx="7222420" cy="2843472"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="1" fPrintsWithSheet="1"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic macro="" fPublished="0">
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="그림 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1343024" y="15725777"/>
+          <a:ext cx="7177087" cy="2904565"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="1" fPrintsWithSheet="1"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic macro="" fPublished="0">
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="그림 30"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1365691" y="18635924"/>
+          <a:ext cx="7177087" cy="2812812"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1613,10 +1710,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheetPr codeName="Sheet1"/>
-  <x:dimension ref="B2:O42"/>
+  <x:dimension ref="B2:O74"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <x:selection activeCell="S4" activeCellId="0" sqref="S4:S4"/>
+    <x:sheetView tabSelected="1" topLeftCell="B46" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <x:selection activeCell="K79" activeCellId="0" sqref="K79:K79"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="16.39999999999999857891"/>
@@ -1669,7 +1766,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="F3" s="4" t="s">
-        <x:v>1</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="G3" s="4" t="s">
         <x:v>20</x:v>
@@ -1687,7 +1784,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="L3" s="4" t="s">
-        <x:v>2</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="M3" s="4" t="s">
         <x:v>12</x:v>
@@ -1707,7 +1804,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="D4" s="2" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E4" s="2">
         <x:v>30</x:v>
@@ -1719,7 +1816,7 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="H4" s="28" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="I4" s="2" t="s">
         <x:v>0</x:v>
@@ -1731,13 +1828,13 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="L4" s="2" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="M4" s="2" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N4" s="7" t="s">
-        <x:v>3</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="O4" s="18">
         <x:v>0.98069999999999991</x:v>
@@ -1751,7 +1848,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="D5" s="2" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E5" s="2">
         <x:v>30</x:v>
@@ -1763,7 +1860,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="H5" s="28" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="I5" s="2" t="s">
         <x:v>0</x:v>
@@ -1775,13 +1872,13 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="L5" s="2" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="M5" s="2" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N5" s="7" t="s">
-        <x:v>4</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="O5" s="18">
         <x:v>0.97989999999999999</x:v>
@@ -1795,7 +1892,7 @@
         <x:v>64</x:v>
       </x:c>
       <x:c r="D6" s="2" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="E6" s="2">
         <x:v>30</x:v>
@@ -1807,7 +1904,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="H6" s="28" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="I6" s="2" t="s">
         <x:v>0</x:v>
@@ -1822,13 +1919,13 @@
         <x:v>0.5</x:v>
       </x:c>
       <x:c r="M6" s="2" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="N6" s="7" t="s">
-        <x:v>4</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="O6" s="18">
-        <x:v>0.97989999999999999</x:v>
+        <x:v>0.98060000000000003</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="2:15">
@@ -1928,8 +2025,8 @@
       <x:c r="O12" s="1"/>
     </x:row>
     <x:row r="13" spans="2:15" ht="15.75" customHeight="1">
-      <x:c r="B13" s="29" t="s">
-        <x:v>5</x:v>
+      <x:c r="B13" s="35" t="s">
+        <x:v>26</x:v>
       </x:c>
       <x:c r="C13" s="30"/>
       <x:c r="D13" s="30"/>
@@ -2232,6 +2329,11 @@
         <x:v>23</x:v>
       </x:c>
     </x:row>
+    <x:row r="74" spans="4:4">
+      <x:c r="D74" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:mergeCells count="3">
     <x:mergeCell ref="B2:O2"/>

</xml_diff>